<commit_message>
Corrected xlsx with new bMean columns
</commit_message>
<xml_diff>
--- a/QPPh_microstruct.xlsx
+++ b/QPPh_microstruct.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabie\Desktop\Licking paper\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A27D655-5A82-4AD1-AA05-9E5876B8C68A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{7A24416D-9519-4AB2-9E06-526242DA6DCB}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22785" windowHeight="14655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$T$98</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="28">
   <si>
     <t>QPPh1.01</t>
   </si>
@@ -112,11 +106,17 @@
   <si>
     <t>Free choice malto</t>
   </si>
+  <si>
+    <t>By Session</t>
+  </si>
+  <si>
+    <t>By Rat</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +178,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -191,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -214,12 +226,20 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -520,31 +540,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5314A094-4845-4879-ACDA-569370418266}">
-  <dimension ref="A1:AI98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="480" activePane="bottomLeft"/>
       <selection activeCell="AM1" sqref="AM1:AS1048576"/>
-      <selection pane="bottomLeft" activeCell="AP17" sqref="AP17"/>
+      <selection pane="bottomLeft" activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="I1" s="13" t="s">
         <v>22</v>
       </c>
@@ -578,7 +599,7 @@
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
     </row>
-    <row r="2" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
@@ -670,7 +691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -729,7 +750,7 @@
         <v>561</v>
       </c>
       <c r="X3">
-        <v>17.387096774193498</v>
+        <v>10.545454545454501</v>
       </c>
       <c r="Y3">
         <v>11</v>
@@ -747,7 +768,7 @@
         <v>142</v>
       </c>
       <c r="AD3">
-        <v>10.346153846153801</v>
+        <v>24.6538461538461</v>
       </c>
       <c r="AE3">
         <v>21</v>
@@ -765,7 +786,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -824,7 +845,7 @@
         <v>611</v>
       </c>
       <c r="X4">
-        <v>19.818181818181799</v>
+        <v>14.3333333333333</v>
       </c>
       <c r="Y4">
         <v>15</v>
@@ -842,7 +863,7 @@
         <v>229</v>
       </c>
       <c r="AD4">
-        <v>15.3846153846153</v>
+        <v>13.2558139534883</v>
       </c>
       <c r="AE4">
         <v>30</v>
@@ -860,7 +881,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -919,7 +940,7 @@
         <v>459</v>
       </c>
       <c r="X5">
-        <v>8.3673469387755102</v>
+        <v>7.2307692307692299</v>
       </c>
       <c r="Y5">
         <v>13</v>
@@ -937,7 +958,7 @@
         <v>96</v>
       </c>
       <c r="AD5">
-        <v>3.578125</v>
+        <v>5.75</v>
       </c>
       <c r="AE5">
         <v>100</v>
@@ -955,7 +976,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1014,7 +1035,7 @@
         <v>584</v>
       </c>
       <c r="X6">
-        <v>8.75</v>
+        <v>16</v>
       </c>
       <c r="Y6">
         <v>2</v>
@@ -1032,7 +1053,7 @@
         <v>49</v>
       </c>
       <c r="AD6">
-        <v>4.5702479338842901</v>
+        <v>11.24</v>
       </c>
       <c r="AE6">
         <v>54</v>
@@ -1050,7 +1071,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1109,7 +1130,7 @@
         <v>588</v>
       </c>
       <c r="X7">
-        <v>14.789473684210501</v>
+        <v>14</v>
       </c>
       <c r="Y7">
         <v>26</v>
@@ -1127,7 +1148,7 @@
         <v>387</v>
       </c>
       <c r="AD7">
-        <v>14.5</v>
+        <v>20.2903225806451</v>
       </c>
       <c r="AE7">
         <v>5</v>
@@ -1145,7 +1166,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1204,7 +1225,7 @@
         <v>620</v>
       </c>
       <c r="X8">
-        <v>26.08</v>
+        <v>14.5</v>
       </c>
       <c r="Y8">
         <v>4</v>
@@ -1222,7 +1243,7 @@
         <v>88</v>
       </c>
       <c r="AD8">
-        <v>15.179487179487101</v>
+        <v>23.727272727272702</v>
       </c>
       <c r="AE8">
         <v>33</v>
@@ -1240,7 +1261,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1299,7 +1320,7 @@
         <v>669</v>
       </c>
       <c r="X9">
-        <v>10.2456140350877</v>
+        <v>10</v>
       </c>
       <c r="Y9">
         <v>2</v>
@@ -1317,7 +1338,7 @@
         <v>27</v>
       </c>
       <c r="AD9">
-        <v>16</v>
+        <v>11.8125</v>
       </c>
       <c r="AE9">
         <v>42</v>
@@ -1335,7 +1356,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1394,7 +1415,7 @@
         <v>543</v>
       </c>
       <c r="X10">
-        <v>13.8734177215189</v>
+        <v>21</v>
       </c>
       <c r="Y10">
         <v>1</v>
@@ -1412,7 +1433,7 @@
         <v>28</v>
       </c>
       <c r="AD10">
-        <v>5.2727272727272698</v>
+        <v>11.714285714285699</v>
       </c>
       <c r="AE10">
         <v>100</v>
@@ -1430,7 +1451,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1489,7 +1510,7 @@
         <v>509</v>
       </c>
       <c r="X11">
-        <v>15.9189189189189</v>
+        <v>18.3</v>
       </c>
       <c r="Y11">
         <v>10</v>
@@ -1507,7 +1528,7 @@
         <v>210</v>
       </c>
       <c r="AD11">
-        <v>12.2682926829268</v>
+        <v>25.409090909090899</v>
       </c>
       <c r="AE11">
         <v>16</v>
@@ -1525,7 +1546,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1584,7 +1605,7 @@
         <v>569</v>
       </c>
       <c r="X12">
-        <v>21.75</v>
+        <v>9.05555555555555</v>
       </c>
       <c r="Y12">
         <v>36</v>
@@ -1602,7 +1623,7 @@
         <v>358</v>
       </c>
       <c r="AD12">
-        <v>7.8888888888888804</v>
+        <v>20.321428571428498</v>
       </c>
       <c r="AE12">
         <v>11</v>
@@ -1620,7 +1641,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1679,7 +1700,7 @@
         <v>696</v>
       </c>
       <c r="X13">
-        <v>13.232558139534801</v>
+        <v>8.7777777777777697</v>
       </c>
       <c r="Y13">
         <v>18</v>
@@ -1697,7 +1718,7 @@
         <v>160</v>
       </c>
       <c r="AD13">
-        <v>14.7777777777777</v>
+        <v>12.7083333333333</v>
       </c>
       <c r="AE13">
         <v>30</v>
@@ -1715,7 +1736,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1774,7 +1795,7 @@
         <v>551</v>
       </c>
       <c r="X14">
-        <v>5.0714285714285703</v>
+        <v>6.4193548387096699</v>
       </c>
       <c r="Y14">
         <v>31</v>
@@ -1792,7 +1813,7 @@
         <v>214</v>
       </c>
       <c r="AD14">
-        <v>3.5424836601307099</v>
+        <v>15.7777777777777</v>
       </c>
       <c r="AE14">
         <v>100</v>
@@ -1810,7 +1831,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1869,7 +1890,7 @@
         <v>550</v>
       </c>
       <c r="X15">
-        <v>18.5483870967741</v>
+        <v>12.4</v>
       </c>
       <c r="Y15">
         <v>10</v>
@@ -1887,7 +1908,7 @@
         <v>149</v>
       </c>
       <c r="AD15">
-        <v>16.40625</v>
+        <v>15.5365853658536</v>
       </c>
       <c r="AE15">
         <v>31</v>
@@ -1905,7 +1926,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1964,7 +1985,7 @@
         <v>971</v>
       </c>
       <c r="X16">
-        <v>22.571428571428498</v>
+        <v>20.318181818181799</v>
       </c>
       <c r="Y16">
         <v>22</v>
@@ -1982,7 +2003,7 @@
         <v>475</v>
       </c>
       <c r="AD16">
-        <v>24.473684210526301</v>
+        <v>14.2</v>
       </c>
       <c r="AE16">
         <v>5</v>
@@ -2000,7 +2021,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -2059,7 +2080,7 @@
         <v>646</v>
       </c>
       <c r="X17">
-        <v>4.4516129032257998</v>
+        <v>4.3170731707316996</v>
       </c>
       <c r="Y17">
         <v>41</v>
@@ -2077,7 +2098,7 @@
         <v>189</v>
       </c>
       <c r="AD17">
-        <v>10.174603174603099</v>
+        <v>9.4722222222222197</v>
       </c>
       <c r="AE17">
         <v>36</v>
@@ -2095,7 +2116,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -2154,7 +2175,7 @@
         <v>565</v>
       </c>
       <c r="X18">
-        <v>5.1571428571428504</v>
+        <v>3</v>
       </c>
       <c r="Y18">
         <v>1</v>
@@ -2172,7 +2193,7 @@
         <v>13</v>
       </c>
       <c r="AD18">
-        <v>4.1167883211678804</v>
+        <v>10.233333333333301</v>
       </c>
       <c r="AE18">
         <v>185</v>
@@ -2190,7 +2211,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -2249,7 +2270,7 @@
         <v>547</v>
       </c>
       <c r="X19">
-        <v>24.782608695652101</v>
+        <v>18.952380952380899</v>
       </c>
       <c r="Y19">
         <v>21</v>
@@ -2267,7 +2288,7 @@
         <v>425</v>
       </c>
       <c r="AD19">
-        <v>11.782608695652099</v>
+        <v>30.2</v>
       </c>
       <c r="AE19">
         <v>6</v>
@@ -2285,7 +2306,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -2344,7 +2365,7 @@
         <v>620</v>
       </c>
       <c r="X20">
-        <v>18.03125</v>
+        <v>14.8888888888888</v>
       </c>
       <c r="Y20">
         <v>27</v>
@@ -2362,7 +2383,7 @@
         <v>431</v>
       </c>
       <c r="AD20">
-        <v>19.0322580645161</v>
+        <v>19.931034482758601</v>
       </c>
       <c r="AE20">
         <v>4</v>
@@ -2380,7 +2401,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -2439,7 +2460,7 @@
         <v>665</v>
       </c>
       <c r="X21">
-        <v>12.6875</v>
+        <v>4.1111111111111098</v>
       </c>
       <c r="Y21">
         <v>9</v>
@@ -2457,7 +2478,7 @@
         <v>66</v>
       </c>
       <c r="AD21">
-        <v>13.25</v>
+        <v>30.785714285714199</v>
       </c>
       <c r="AE21">
         <v>44</v>
@@ -2475,7 +2496,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -2534,7 +2555,7 @@
         <v>596</v>
       </c>
       <c r="X22">
-        <v>12.6458333333333</v>
+        <v>10.4</v>
       </c>
       <c r="Y22">
         <v>5</v>
@@ -2552,7 +2573,7 @@
         <v>54</v>
       </c>
       <c r="AD22">
-        <v>7.7808219178082103</v>
+        <v>4.3076923076923004</v>
       </c>
       <c r="AE22">
         <v>63</v>
@@ -2570,7 +2591,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -2629,7 +2650,7 @@
         <v>567</v>
       </c>
       <c r="X23">
-        <v>15.45</v>
+        <v>9.86666666666666</v>
       </c>
       <c r="Y23">
         <v>30</v>
@@ -2647,7 +2668,7 @@
         <v>310</v>
       </c>
       <c r="AD23">
-        <v>13.9743589743589</v>
+        <v>26.55</v>
       </c>
       <c r="AE23">
         <v>11</v>
@@ -2665,7 +2686,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -2724,7 +2745,7 @@
         <v>641</v>
       </c>
       <c r="X24">
-        <v>18.1142857142857</v>
+        <v>16.2916666666666</v>
       </c>
       <c r="Y24">
         <v>24</v>
@@ -2742,7 +2763,7 @@
         <v>423</v>
       </c>
       <c r="AD24">
-        <v>21.857142857142801</v>
+        <v>21.535714285714199</v>
       </c>
       <c r="AE24">
         <v>9</v>
@@ -2760,7 +2781,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
@@ -2819,7 +2840,7 @@
         <v>660</v>
       </c>
       <c r="X25">
-        <v>9.8983050847457594</v>
+        <v>13.6</v>
       </c>
       <c r="Y25">
         <v>5</v>
@@ -2837,7 +2858,7 @@
         <v>80</v>
       </c>
       <c r="AD25">
-        <v>15.023809523809501</v>
+        <v>11.5555555555555</v>
       </c>
       <c r="AE25">
         <v>31</v>
@@ -2855,7 +2876,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -2914,7 +2935,7 @@
         <v>584</v>
       </c>
       <c r="X26">
-        <v>4.5168539325842696</v>
+        <v>0</v>
       </c>
       <c r="Y26">
         <v>0</v>
@@ -2932,7 +2953,7 @@
         <v>0</v>
       </c>
       <c r="AD26">
-        <v>6.5</v>
+        <v>10.1111111111111</v>
       </c>
       <c r="AE26">
         <v>85</v>
@@ -2950,7 +2971,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -3009,7 +3030,7 @@
         <v>561</v>
       </c>
       <c r="X27">
-        <v>7.3235294117647003</v>
+        <v>8.4761904761904692</v>
       </c>
       <c r="Y27">
         <v>21</v>
@@ -3027,7 +3048,7 @@
         <v>189</v>
       </c>
       <c r="AD27">
-        <v>13.8</v>
+        <v>26.28</v>
       </c>
       <c r="AE27">
         <v>22</v>
@@ -3045,7 +3066,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
@@ -3104,7 +3125,7 @@
         <v>581</v>
       </c>
       <c r="X28">
-        <v>15.8157894736842</v>
+        <v>14.863636363636299</v>
       </c>
       <c r="Y28">
         <v>22</v>
@@ -3122,7 +3143,7 @@
         <v>346</v>
       </c>
       <c r="AD28">
-        <v>12.244444444444399</v>
+        <v>14.5142857142857</v>
       </c>
       <c r="AE28">
         <v>17</v>
@@ -3140,7 +3161,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -3199,7 +3220,7 @@
         <v>665</v>
       </c>
       <c r="X29">
-        <v>8.5492957746478808</v>
+        <v>11.6666666666666</v>
       </c>
       <c r="Y29">
         <v>3</v>
@@ -3217,7 +3238,7 @@
         <v>57</v>
       </c>
       <c r="AD29">
-        <v>16.282051282051199</v>
+        <v>8.1578947368421009</v>
       </c>
       <c r="AE29">
         <v>36</v>
@@ -3235,7 +3256,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -3294,7 +3315,7 @@
         <v>580</v>
       </c>
       <c r="X30">
-        <v>8.5932203389830502</v>
+        <v>6</v>
       </c>
       <c r="Y30">
         <v>8</v>
@@ -3312,7 +3333,7 @@
         <v>64</v>
       </c>
       <c r="AD30">
-        <v>6.0744680851063801</v>
+        <v>13.2758620689655</v>
       </c>
       <c r="AE30">
         <v>67</v>
@@ -3330,7 +3351,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -3389,7 +3410,7 @@
         <v>595</v>
       </c>
       <c r="X31">
-        <v>10.1960784313725</v>
+        <v>7.9047619047618998</v>
       </c>
       <c r="Y31">
         <v>21</v>
@@ -3407,7 +3428,7 @@
         <v>184</v>
       </c>
       <c r="AD31">
-        <v>16.735294117647001</v>
+        <v>26.0833333333333</v>
       </c>
       <c r="AE31">
         <v>19</v>
@@ -3425,7 +3446,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -3484,7 +3505,7 @@
         <v>554</v>
       </c>
       <c r="X32">
-        <v>12.7254901960784</v>
+        <v>11.75</v>
       </c>
       <c r="Y32">
         <v>28</v>
@@ -3502,7 +3523,7 @@
         <v>358</v>
       </c>
       <c r="AD32">
-        <v>15.6</v>
+        <v>21.6538461538461</v>
       </c>
       <c r="AE32">
         <v>10</v>
@@ -3520,7 +3541,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
@@ -3579,7 +3600,7 @@
         <v>716</v>
       </c>
       <c r="X33">
-        <v>11.207547169811299</v>
+        <v>0</v>
       </c>
       <c r="Y33">
         <v>0</v>
@@ -3597,7 +3618,7 @@
         <v>0</v>
       </c>
       <c r="AD33">
-        <v>16.3095238095238</v>
+        <v>5.8250000000000002</v>
       </c>
       <c r="AE33">
         <v>38</v>
@@ -3615,7 +3636,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -3674,7 +3695,7 @@
         <v>553</v>
       </c>
       <c r="X34">
-        <v>5.9756097560975601</v>
+        <v>0</v>
       </c>
       <c r="Y34">
         <v>0</v>
@@ -3692,7 +3713,7 @@
         <v>0</v>
       </c>
       <c r="AD34">
-        <v>6.0786516853932504</v>
+        <v>10.8</v>
       </c>
       <c r="AE34">
         <v>88</v>
@@ -3710,7 +3731,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -3769,7 +3790,7 @@
         <v>538</v>
       </c>
       <c r="X35">
-        <v>1.6216216216216199</v>
+        <v>0</v>
       </c>
       <c r="Y35">
         <v>0</v>
@@ -3787,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="AD35">
-        <v>12.465116279069701</v>
+        <v>24.08</v>
       </c>
       <c r="AE35">
         <v>36</v>
@@ -3805,7 +3826,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
@@ -3864,7 +3885,7 @@
         <v>570</v>
       </c>
       <c r="X36">
-        <v>1.88888888888888</v>
+        <v>4.4153846153846104</v>
       </c>
       <c r="Y36">
         <v>65</v>
@@ -3882,7 +3903,7 @@
         <v>288</v>
       </c>
       <c r="AD36">
-        <v>20.925925925925899</v>
+        <v>0</v>
       </c>
       <c r="AE36">
         <v>14</v>
@@ -3900,7 +3921,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -3959,7 +3980,7 @@
         <v>551</v>
       </c>
       <c r="X37">
-        <v>3.7555555555555502</v>
+        <v>0</v>
       </c>
       <c r="Y37">
         <v>0</v>
@@ -3977,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="AD37">
-        <v>7.7464788732394299</v>
+        <v>3.0925925925925899</v>
       </c>
       <c r="AE37">
         <v>45</v>
@@ -3995,7 +4016,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
@@ -4054,7 +4075,7 @@
         <v>761</v>
       </c>
       <c r="X38">
-        <v>2.0581395348837201</v>
+        <v>0</v>
       </c>
       <c r="Y38">
         <v>0</v>
@@ -4072,7 +4093,7 @@
         <v>0</v>
       </c>
       <c r="AD38">
-        <v>16.177777777777699</v>
+        <v>2.5529411764705801</v>
       </c>
       <c r="AE38">
         <v>42</v>
@@ -4090,7 +4111,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -4149,7 +4170,7 @@
         <v>550</v>
       </c>
       <c r="X39">
-        <v>2.7179487179487101</v>
+        <v>0</v>
       </c>
       <c r="Y39">
         <v>0</v>
@@ -4167,7 +4188,7 @@
         <v>0</v>
       </c>
       <c r="AD39">
-        <v>12.177777777777701</v>
+        <v>30.315789473684202</v>
       </c>
       <c r="AE39">
         <v>36</v>
@@ -4185,7 +4206,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>1</v>
       </c>
@@ -4244,7 +4265,7 @@
         <v>507</v>
       </c>
       <c r="X40">
-        <v>10.818181818181801</v>
+        <v>7.2439024390243896</v>
       </c>
       <c r="Y40">
         <v>41</v>
@@ -4262,7 +4283,7 @@
         <v>315</v>
       </c>
       <c r="AD40">
-        <v>19.96</v>
+        <v>7.0270270270270201</v>
       </c>
       <c r="AE40">
         <v>14</v>
@@ -4280,7 +4301,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>6</v>
       </c>
@@ -4339,7 +4360,7 @@
         <v>686</v>
       </c>
       <c r="X41">
-        <v>9.0847457627118597</v>
+        <v>3.5</v>
       </c>
       <c r="Y41">
         <v>6</v>
@@ -4357,7 +4378,7 @@
         <v>22</v>
       </c>
       <c r="AD41">
-        <v>12.4</v>
+        <v>2.6818181818181799</v>
       </c>
       <c r="AE41">
         <v>50</v>
@@ -4375,7 +4396,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
@@ -4434,7 +4455,7 @@
         <v>670</v>
       </c>
       <c r="X42">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Y42">
         <v>0</v>
@@ -4452,7 +4473,7 @@
         <v>0</v>
       </c>
       <c r="AD42">
-        <v>10.4603174603174</v>
+        <v>7.7948717948717903</v>
       </c>
       <c r="AE42">
         <v>55</v>
@@ -4470,7 +4491,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -4529,7 +4550,7 @@
         <v>527</v>
       </c>
       <c r="X43">
-        <v>1.5333333333333301</v>
+        <v>0</v>
       </c>
       <c r="Y43">
         <v>0</v>
@@ -4547,7 +4568,7 @@
         <v>0</v>
       </c>
       <c r="AD43">
-        <v>11.6666666666666</v>
+        <v>16.3</v>
       </c>
       <c r="AE43">
         <v>36</v>
@@ -4565,7 +4586,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>1</v>
       </c>
@@ -4640,7 +4661,7 @@
         <v>0</v>
       </c>
       <c r="AD44">
-        <v>10.372881355932201</v>
+        <v>6.3636363636363598</v>
       </c>
       <c r="AE44">
         <v>29</v>
@@ -4658,7 +4679,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>6</v>
       </c>
@@ -4717,7 +4738,7 @@
         <v>521</v>
       </c>
       <c r="X45">
-        <v>5.4375</v>
+        <v>0</v>
       </c>
       <c r="Y45">
         <v>0</v>
@@ -4735,7 +4756,7 @@
         <v>0</v>
       </c>
       <c r="AD45">
-        <v>3.96946564885496</v>
+        <v>0</v>
       </c>
       <c r="AE45">
         <v>111</v>
@@ -4753,7 +4774,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -4812,7 +4833,7 @@
         <v>511</v>
       </c>
       <c r="X46">
-        <v>1.8571428571428501</v>
+        <v>0</v>
       </c>
       <c r="Y46">
         <v>0</v>
@@ -4830,7 +4851,7 @@
         <v>0</v>
       </c>
       <c r="AD46">
-        <v>4.9223300970873698</v>
+        <v>4</v>
       </c>
       <c r="AE46">
         <v>59</v>
@@ -4848,7 +4869,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -4907,7 +4928,7 @@
         <v>370</v>
       </c>
       <c r="X47">
-        <v>1.6666666666666601</v>
+        <v>0</v>
       </c>
       <c r="Y47">
         <v>0</v>
@@ -4925,7 +4946,7 @@
         <v>0</v>
       </c>
       <c r="AD47">
-        <v>21.058823529411701</v>
+        <v>23.625</v>
       </c>
       <c r="AE47">
         <v>21</v>
@@ -4943,7 +4964,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>1</v>
       </c>
@@ -5002,7 +5023,7 @@
         <v>579</v>
       </c>
       <c r="X48">
-        <v>4.2380952380952301</v>
+        <v>4.1410256410256396</v>
       </c>
       <c r="Y48">
         <v>78</v>
@@ -5020,7 +5041,7 @@
         <v>337</v>
       </c>
       <c r="AD48">
-        <v>24.772727272727199</v>
+        <v>5.6590909090909003</v>
       </c>
       <c r="AE48">
         <v>13</v>
@@ -5038,7 +5059,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>6</v>
       </c>
@@ -5097,7 +5118,7 @@
         <v>702</v>
       </c>
       <c r="X49">
-        <v>6.9024390243902403</v>
+        <v>0</v>
       </c>
       <c r="Y49">
         <v>0</v>
@@ -5115,7 +5136,7 @@
         <v>0</v>
       </c>
       <c r="AD49">
-        <v>18.6666666666666</v>
+        <v>14.1785714285714</v>
       </c>
       <c r="AE49">
         <v>37</v>
@@ -5133,7 +5154,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
@@ -5192,7 +5213,7 @@
         <v>650</v>
       </c>
       <c r="X50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Y50">
         <v>0</v>
@@ -5210,7 +5231,7 @@
         <v>0</v>
       </c>
       <c r="AD50">
-        <v>8.1898734177215093</v>
+        <v>4.6818181818181799</v>
       </c>
       <c r="AE50">
         <v>54</v>
@@ -5228,7 +5249,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>2</v>
       </c>
@@ -5287,7 +5308,7 @@
         <v>660</v>
       </c>
       <c r="X51">
-        <v>34.090909090909001</v>
+        <v>14</v>
       </c>
       <c r="Y51">
         <v>26</v>
@@ -5305,7 +5326,7 @@
         <v>675</v>
       </c>
       <c r="AD51">
-        <v>7.9146341463414602</v>
+        <v>0</v>
       </c>
       <c r="AE51">
         <v>0</v>
@@ -5323,7 +5344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>3</v>
       </c>
@@ -5382,7 +5403,7 @@
         <v>428</v>
       </c>
       <c r="X52">
-        <v>23.28125</v>
+        <v>9.43333333333333</v>
       </c>
       <c r="Y52">
         <v>43</v>
@@ -5400,7 +5421,7 @@
         <v>604</v>
       </c>
       <c r="AD52">
-        <v>7.8703703703703702</v>
+        <v>2.5</v>
       </c>
       <c r="AE52">
         <v>6</v>
@@ -5418,7 +5439,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>4</v>
       </c>
@@ -5477,7 +5498,7 @@
         <v>734</v>
       </c>
       <c r="X53">
-        <v>7.3624999999999998</v>
+        <v>3.2</v>
       </c>
       <c r="Y53">
         <v>40</v>
@@ -5495,7 +5516,7 @@
         <v>233</v>
       </c>
       <c r="AD53">
-        <v>25.035714285714199</v>
+        <v>18.8888888888888</v>
       </c>
       <c r="AE53">
         <v>18</v>
@@ -5513,7 +5534,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
@@ -5572,7 +5593,7 @@
         <v>649</v>
       </c>
       <c r="X54">
-        <v>4.1414141414141401</v>
+        <v>9.2962962962962905</v>
       </c>
       <c r="Y54">
         <v>25</v>
@@ -5590,7 +5611,7 @@
         <v>286</v>
       </c>
       <c r="AD54">
-        <v>16.615384615384599</v>
+        <v>15.5833333333333</v>
       </c>
       <c r="AE54">
         <v>12</v>
@@ -5608,7 +5629,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>2</v>
       </c>
@@ -5667,7 +5688,7 @@
         <v>751</v>
       </c>
       <c r="X55">
-        <v>31.391304347826001</v>
+        <v>20.6</v>
       </c>
       <c r="Y55">
         <v>31</v>
@@ -5685,7 +5706,7 @@
         <v>664</v>
       </c>
       <c r="AD55">
-        <v>23.4838709677419</v>
+        <v>0</v>
       </c>
       <c r="AE55">
         <v>0</v>
@@ -5703,7 +5724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>3</v>
       </c>
@@ -5762,7 +5783,7 @@
         <v>358</v>
       </c>
       <c r="X56">
-        <v>23.3333333333333</v>
+        <v>13.272727272727201</v>
       </c>
       <c r="Y56">
         <v>11</v>
@@ -5780,7 +5801,7 @@
         <v>264</v>
       </c>
       <c r="AD56">
-        <v>4.9295774647887303</v>
+        <v>4.7777777777777697</v>
       </c>
       <c r="AE56">
         <v>9</v>
@@ -5798,7 +5819,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>4</v>
       </c>
@@ -5857,7 +5878,7 @@
         <v>706</v>
       </c>
       <c r="X57">
-        <v>16.707317073170699</v>
+        <v>12.8095238095238</v>
       </c>
       <c r="Y57">
         <v>32</v>
@@ -5875,7 +5896,7 @@
         <v>396</v>
       </c>
       <c r="AD57">
-        <v>21.838709677419299</v>
+        <v>8.3157894736842106</v>
       </c>
       <c r="AE57">
         <v>19</v>
@@ -5893,7 +5914,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>5</v>
       </c>
@@ -5952,7 +5973,7 @@
         <v>686</v>
       </c>
       <c r="X58">
-        <v>10.735294117646999</v>
+        <v>4.66</v>
       </c>
       <c r="Y58">
         <v>7</v>
@@ -5970,7 +5991,7 @@
         <v>106</v>
       </c>
       <c r="AD58">
-        <v>17.564102564102502</v>
+        <v>12.25</v>
       </c>
       <c r="AE58">
         <v>28</v>
@@ -5988,7 +6009,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>2</v>
       </c>
@@ -6047,7 +6068,7 @@
         <v>732</v>
       </c>
       <c r="X59">
-        <v>26.884615384615302</v>
+        <v>17.9375</v>
       </c>
       <c r="Y59">
         <v>22</v>
@@ -6065,7 +6086,7 @@
         <v>593</v>
       </c>
       <c r="AD59">
-        <v>26.107142857142801</v>
+        <v>34</v>
       </c>
       <c r="AE59">
         <v>1</v>
@@ -6083,7 +6104,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>3</v>
       </c>
@@ -6142,7 +6163,7 @@
         <v>619</v>
       </c>
       <c r="X60">
-        <v>24.6551724137931</v>
+        <v>19.272727272727199</v>
       </c>
       <c r="Y60">
         <v>28</v>
@@ -6160,7 +6181,7 @@
         <v>602</v>
       </c>
       <c r="AD60">
-        <v>10.4237288135593</v>
+        <v>10.5</v>
       </c>
       <c r="AE60">
         <v>2</v>
@@ -6178,7 +6199,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>4</v>
       </c>
@@ -6237,7 +6258,7 @@
         <v>785</v>
       </c>
       <c r="X61">
-        <v>13.3</v>
+        <v>12.9</v>
       </c>
       <c r="Y61">
         <v>24</v>
@@ -6255,7 +6276,7 @@
         <v>325</v>
       </c>
       <c r="AD61">
-        <v>27.814814814814799</v>
+        <v>26.8</v>
       </c>
       <c r="AE61">
         <v>10</v>
@@ -6273,7 +6294,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>5</v>
       </c>
@@ -6332,7 +6353,7 @@
         <v>612</v>
       </c>
       <c r="X62">
-        <v>11.930232558139499</v>
+        <v>2.31</v>
       </c>
       <c r="Y62">
         <v>27</v>
@@ -6350,7 +6371,7 @@
         <v>428</v>
       </c>
       <c r="AD62">
-        <v>16.078947368421002</v>
+        <v>14</v>
       </c>
       <c r="AE62">
         <v>2</v>
@@ -6368,7 +6389,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>2</v>
       </c>
@@ -6427,7 +6448,7 @@
         <v>720</v>
       </c>
       <c r="X63">
-        <v>22.484848484848399</v>
+        <v>10.6451612903225</v>
       </c>
       <c r="Y63">
         <v>41</v>
@@ -6445,7 +6466,7 @@
         <v>640</v>
       </c>
       <c r="AD63">
-        <v>28.7083333333333</v>
+        <v>0</v>
       </c>
       <c r="AE63">
         <v>0</v>
@@ -6463,7 +6484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>3</v>
       </c>
@@ -6522,7 +6543,7 @@
         <v>536</v>
       </c>
       <c r="X64">
-        <v>22.774193548387</v>
+        <v>16.8</v>
       </c>
       <c r="Y64">
         <v>35</v>
@@ -6540,7 +6561,7 @@
         <v>528</v>
       </c>
       <c r="AD64">
-        <v>8.1060606060606002</v>
+        <v>19</v>
       </c>
       <c r="AE64">
         <v>1</v>
@@ -6558,7 +6579,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>4</v>
       </c>
@@ -6617,7 +6638,7 @@
         <v>771</v>
       </c>
       <c r="X65">
-        <v>7.8831168831168803</v>
+        <v>9.2777777777777697</v>
       </c>
       <c r="Y65">
         <v>36</v>
@@ -6635,7 +6656,7 @@
         <v>350</v>
       </c>
       <c r="AD65">
-        <v>22.303030303030301</v>
+        <v>21.545454545454501</v>
       </c>
       <c r="AE65">
         <v>11</v>
@@ -6653,7 +6674,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>5</v>
       </c>
@@ -6712,7 +6733,7 @@
         <v>625</v>
       </c>
       <c r="X66">
-        <v>7.55</v>
+        <v>2.14054054054054</v>
       </c>
       <c r="Y66">
         <v>30</v>
@@ -6730,7 +6751,7 @@
         <v>331</v>
       </c>
       <c r="AD66">
-        <v>18.909090909090899</v>
+        <v>15.5</v>
       </c>
       <c r="AE66">
         <v>6</v>
@@ -6748,7 +6769,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>2</v>
       </c>
@@ -6807,7 +6828,7 @@
         <v>716</v>
       </c>
       <c r="X67">
-        <v>25.7777777777777</v>
+        <v>12.1666666666666</v>
       </c>
       <c r="Y67">
         <v>20</v>
@@ -6825,7 +6846,7 @@
         <v>639</v>
       </c>
       <c r="AD67">
-        <v>12.1016949152542</v>
+        <v>0</v>
       </c>
       <c r="AE67">
         <v>0</v>
@@ -6843,7 +6864,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>3</v>
       </c>
@@ -6902,7 +6923,7 @@
         <v>575</v>
       </c>
       <c r="X68">
-        <v>19.617647058823501</v>
+        <v>28</v>
       </c>
       <c r="Y68">
         <v>29</v>
@@ -6920,7 +6941,7 @@
         <v>610</v>
       </c>
       <c r="AD68">
-        <v>9.1803278688524497</v>
+        <v>0</v>
       </c>
       <c r="AE68">
         <v>0</v>
@@ -6938,7 +6959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>4</v>
       </c>
@@ -6997,7 +7018,7 @@
         <v>701</v>
       </c>
       <c r="X69">
-        <v>17.375</v>
+        <v>11.2045454545454</v>
       </c>
       <c r="Y69">
         <v>14</v>
@@ -7015,7 +7036,7 @@
         <v>464</v>
       </c>
       <c r="AD69">
-        <v>20.8125</v>
+        <v>23.285714285714199</v>
       </c>
       <c r="AE69">
         <v>7</v>
@@ -7033,7 +7054,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
@@ -7092,7 +7113,7 @@
         <v>592</v>
       </c>
       <c r="X70">
-        <v>4.2448979591836702</v>
+        <v>7.9365079365079296</v>
       </c>
       <c r="Y70">
         <v>13</v>
@@ -7110,7 +7131,7 @@
         <v>63</v>
       </c>
       <c r="AD70">
-        <v>15.473684210526301</v>
+        <v>11.736842105263101</v>
       </c>
       <c r="AE70">
         <v>19</v>
@@ -7128,7 +7149,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>2</v>
       </c>
@@ -7187,7 +7208,7 @@
         <v>752</v>
       </c>
       <c r="X71">
-        <v>33.545454545454497</v>
+        <v>16.636363636363601</v>
       </c>
       <c r="Y71">
         <v>20</v>
@@ -7205,7 +7226,7 @@
         <v>565</v>
       </c>
       <c r="AD71">
-        <v>27.692307692307601</v>
+        <v>20</v>
       </c>
       <c r="AE71">
         <v>5</v>
@@ -7223,7 +7244,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>3</v>
       </c>
@@ -7282,7 +7303,7 @@
         <v>548</v>
       </c>
       <c r="X72">
-        <v>20.5757575757575</v>
+        <v>15</v>
       </c>
       <c r="Y72">
         <v>28</v>
@@ -7300,7 +7321,7 @@
         <v>624</v>
       </c>
       <c r="AD72">
-        <v>9.3508771929824501</v>
+        <v>0</v>
       </c>
       <c r="AE72">
         <v>0</v>
@@ -7318,7 +7339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>4</v>
       </c>
@@ -7377,7 +7398,7 @@
         <v>761</v>
       </c>
       <c r="X73">
-        <v>14.6086956521739</v>
+        <v>16.580645161290299</v>
       </c>
       <c r="Y73">
         <v>36</v>
@@ -7395,7 +7416,7 @@
         <v>451</v>
       </c>
       <c r="AD73">
-        <v>25.964285714285701</v>
+        <v>28.4</v>
       </c>
       <c r="AE73">
         <v>5</v>
@@ -7413,7 +7434,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>5</v>
       </c>
@@ -7472,7 +7493,7 @@
         <v>584</v>
       </c>
       <c r="X74">
-        <v>7.7222222222222197</v>
+        <v>5.5764705882352903</v>
       </c>
       <c r="Y74">
         <v>18</v>
@@ -7490,7 +7511,7 @@
         <v>184</v>
       </c>
       <c r="AD74">
-        <v>17.6666666666666</v>
+        <v>16.176470588235201</v>
       </c>
       <c r="AE74">
         <v>17</v>
@@ -7508,7 +7529,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>2</v>
       </c>
@@ -7567,7 +7588,7 @@
         <v>737</v>
       </c>
       <c r="X75">
-        <v>28.384615384615302</v>
+        <v>13.1818181818181</v>
       </c>
       <c r="Y75">
         <v>25</v>
@@ -7585,7 +7606,7 @@
         <v>661</v>
       </c>
       <c r="AD75">
-        <v>21.3333333333333</v>
+        <v>0</v>
       </c>
       <c r="AE75">
         <v>0</v>
@@ -7603,7 +7624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>3</v>
       </c>
@@ -7662,7 +7683,7 @@
         <v>630</v>
       </c>
       <c r="X76">
-        <v>25.09375</v>
+        <v>9.5882352941176396</v>
       </c>
       <c r="Y76">
         <v>35</v>
@@ -7680,7 +7701,7 @@
         <v>542</v>
       </c>
       <c r="AD76">
-        <v>13.1041666666666</v>
+        <v>4</v>
       </c>
       <c r="AE76">
         <v>1</v>
@@ -7698,7 +7719,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>4</v>
       </c>
@@ -7757,7 +7778,7 @@
         <v>761</v>
       </c>
       <c r="X77">
-        <v>15.8478260869565</v>
+        <v>15.0277777777777</v>
       </c>
       <c r="Y77">
         <v>57</v>
@@ -7775,7 +7796,7 @@
         <v>469</v>
       </c>
       <c r="AD77">
-        <v>29.12</v>
+        <v>34.6666666666666</v>
       </c>
       <c r="AE77">
         <v>3</v>
@@ -7793,7 +7814,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>5</v>
       </c>
@@ -7852,7 +7873,7 @@
         <v>570</v>
       </c>
       <c r="X78">
-        <v>14.0731707317073</v>
+        <v>6.8208955223880601</v>
       </c>
       <c r="Y78">
         <v>29</v>
@@ -7870,7 +7891,7 @@
         <v>403</v>
       </c>
       <c r="AD78">
-        <v>16</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="AE78">
         <v>5</v>
@@ -7888,7 +7909,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>2</v>
       </c>
@@ -7947,7 +7968,7 @@
         <v>774</v>
       </c>
       <c r="X79">
-        <v>30.956521739130402</v>
+        <v>14.684210526315701</v>
       </c>
       <c r="Y79">
         <v>24</v>
@@ -7965,7 +7986,7 @@
         <v>660</v>
       </c>
       <c r="AD79">
-        <v>18.5</v>
+        <v>0</v>
       </c>
       <c r="AE79">
         <v>0</v>
@@ -7983,7 +8004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:35" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>3</v>
       </c>
@@ -8042,7 +8063,7 @@
         <v>571</v>
       </c>
       <c r="X80">
-        <v>26.034482758620602</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="Y80">
         <v>26</v>
@@ -8060,7 +8081,7 @@
         <v>596</v>
       </c>
       <c r="AD80">
-        <v>8.9682539682539595</v>
+        <v>0</v>
       </c>
       <c r="AE80">
         <v>0</v>
@@ -8078,7 +8099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>4</v>
       </c>
@@ -8137,7 +8158,7 @@
         <v>741</v>
       </c>
       <c r="X81">
-        <v>8.9736842105263097</v>
+        <v>15.8421052631578</v>
       </c>
       <c r="Y81">
         <v>80</v>
@@ -8155,7 +8176,7 @@
         <v>479</v>
       </c>
       <c r="AD81">
-        <v>24.379310344827498</v>
+        <v>11.6666666666666</v>
       </c>
       <c r="AE81">
         <v>3</v>
@@ -8173,7 +8194,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>5</v>
       </c>
@@ -8232,7 +8253,7 @@
         <v>665</v>
       </c>
       <c r="X82">
-        <v>11.255319148936101</v>
+        <v>5.7954545454545396</v>
       </c>
       <c r="Y82">
         <v>30</v>
@@ -8250,7 +8271,7 @@
         <v>340</v>
       </c>
       <c r="AD82">
-        <v>18.4444444444444</v>
+        <v>19</v>
       </c>
       <c r="AE82">
         <v>6</v>
@@ -8268,7 +8289,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>2</v>
       </c>
@@ -8327,7 +8348,7 @@
         <v>710</v>
       </c>
       <c r="X83">
-        <v>14.1224489795918</v>
+        <v>13.0277777777777</v>
       </c>
       <c r="Y83">
         <v>25</v>
@@ -8345,7 +8366,7 @@
         <v>633</v>
       </c>
       <c r="AD83">
-        <v>15.386363636363599</v>
+        <v>0</v>
       </c>
       <c r="AE83">
         <v>0</v>
@@ -8363,7 +8384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>3</v>
       </c>
@@ -8422,7 +8443,7 @@
         <v>589</v>
       </c>
       <c r="X84">
-        <v>6.2045454545454497</v>
+        <v>14.357142857142801</v>
       </c>
       <c r="Y84">
         <v>0</v>
@@ -8440,7 +8461,7 @@
         <v>0</v>
       </c>
       <c r="AD84">
-        <v>11.8163265306122</v>
+        <v>7.8064516129032198</v>
       </c>
       <c r="AE84">
         <v>31</v>
@@ -8458,7 +8479,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>4</v>
       </c>
@@ -8517,7 +8538,7 @@
         <v>750</v>
       </c>
       <c r="X85">
-        <v>6.2525252525252499</v>
+        <v>12.5111111111111</v>
       </c>
       <c r="Y85">
         <v>108</v>
@@ -8535,7 +8556,7 @@
         <v>335</v>
       </c>
       <c r="AD85">
-        <v>26.518518518518501</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AE85">
         <v>5</v>
@@ -8553,7 +8574,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>5</v>
       </c>
@@ -8612,7 +8633,7 @@
         <v>650</v>
       </c>
       <c r="X86">
-        <v>2.7279411764705799</v>
+        <v>14.8809523809523</v>
       </c>
       <c r="Y86">
         <v>85</v>
@@ -8630,7 +8651,7 @@
         <v>222</v>
       </c>
       <c r="AD86">
-        <v>17.5277777777777</v>
+        <v>10.636363636363599</v>
       </c>
       <c r="AE86">
         <v>11</v>
@@ -8648,7 +8669,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>2</v>
       </c>
@@ -8707,7 +8728,7 @@
         <v>741</v>
       </c>
       <c r="X87">
-        <v>18.594594594594501</v>
+        <v>13.3888888888888</v>
       </c>
       <c r="Y87">
         <v>19</v>
@@ -8725,7 +8746,7 @@
         <v>609</v>
       </c>
       <c r="AD87">
-        <v>25.25</v>
+        <v>0</v>
       </c>
       <c r="AE87">
         <v>0</v>
@@ -8743,7 +8764,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>3</v>
       </c>
@@ -8802,7 +8823,7 @@
         <v>590</v>
       </c>
       <c r="X88">
-        <v>7.6</v>
+        <v>16.571428571428498</v>
       </c>
       <c r="Y88">
         <v>37</v>
@@ -8820,7 +8841,7 @@
         <v>278</v>
       </c>
       <c r="AD88">
-        <v>9.3492063492063497</v>
+        <v>7.7</v>
       </c>
       <c r="AE88">
         <v>30</v>
@@ -8838,7 +8859,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>4</v>
       </c>
@@ -8897,7 +8918,7 @@
         <v>780</v>
       </c>
       <c r="X89">
-        <v>6.2840909090909003</v>
+        <v>11.16</v>
       </c>
       <c r="Y89">
         <v>22</v>
@@ -8915,7 +8936,7 @@
         <v>70</v>
       </c>
       <c r="AD89">
-        <v>20.75</v>
+        <v>12.190476190476099</v>
       </c>
       <c r="AE89">
         <v>42</v>
@@ -8933,7 +8954,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="90" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>5</v>
       </c>
@@ -8992,7 +9013,7 @@
         <v>641</v>
       </c>
       <c r="X90">
-        <v>4.1818181818181799</v>
+        <v>11.0363636363636</v>
       </c>
       <c r="Y90">
         <v>39</v>
@@ -9010,7 +9031,7 @@
         <v>310</v>
       </c>
       <c r="AD90">
-        <v>25.625</v>
+        <v>15.375</v>
       </c>
       <c r="AE90">
         <v>8</v>
@@ -9028,7 +9049,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="91" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>2</v>
       </c>
@@ -9087,7 +9108,7 @@
         <v>691</v>
       </c>
       <c r="X91">
-        <v>13.8163265306122</v>
+        <v>13</v>
       </c>
       <c r="Y91">
         <v>20</v>
@@ -9105,7 +9126,7 @@
         <v>358</v>
       </c>
       <c r="AD91">
-        <v>14.3541666666666</v>
+        <v>13.3888888888888</v>
       </c>
       <c r="AE91">
         <v>18</v>
@@ -9123,7 +9144,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="92" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>3</v>
       </c>
@@ -9182,7 +9203,7 @@
         <v>637</v>
       </c>
       <c r="X92">
-        <v>4.7563025210083998</v>
+        <v>13.3793103448275</v>
       </c>
       <c r="Y92">
         <v>33</v>
@@ -9200,7 +9221,7 @@
         <v>212</v>
       </c>
       <c r="AD92">
-        <v>9.4925373134328304</v>
+        <v>5.25</v>
       </c>
       <c r="AE92">
         <v>4</v>
@@ -9218,7 +9239,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>4</v>
       </c>
@@ -9277,7 +9298,7 @@
         <v>652</v>
       </c>
       <c r="X93">
-        <v>3</v>
+        <v>4.1711711711711699</v>
       </c>
       <c r="Y93">
         <v>0</v>
@@ -9295,7 +9316,7 @@
         <v>0</v>
       </c>
       <c r="AD93">
-        <v>6.9042553191489304</v>
+        <v>9.9107142857142794</v>
       </c>
       <c r="AE93">
         <v>56</v>
@@ -9313,7 +9334,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>5</v>
       </c>
@@ -9372,7 +9393,7 @@
         <v>459</v>
       </c>
       <c r="X94">
-        <v>6.8278145695364199</v>
+        <v>8.7796610169491505</v>
       </c>
       <c r="Y94">
         <v>38</v>
@@ -9390,7 +9411,7 @@
         <v>157</v>
       </c>
       <c r="AD94">
-        <v>7.7288135593220302</v>
+        <v>10.4583333333333</v>
       </c>
       <c r="AE94">
         <v>24</v>
@@ -9408,7 +9429,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="95" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>2</v>
       </c>
@@ -9467,7 +9488,7 @@
         <v>794</v>
       </c>
       <c r="X95">
-        <v>29.4583333333333</v>
+        <v>24.8095238095238</v>
       </c>
       <c r="Y95">
         <v>24</v>
@@ -9485,7 +9506,7 @@
         <v>573</v>
       </c>
       <c r="AD95">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AE95">
         <v>1</v>
@@ -9503,7 +9524,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>3</v>
       </c>
@@ -9562,7 +9583,7 @@
         <v>665</v>
       </c>
       <c r="X96">
-        <v>9.4861111111111107</v>
+        <v>11.2307692307692</v>
       </c>
       <c r="Y96">
         <v>44</v>
@@ -9580,7 +9601,7 @@
         <v>270</v>
       </c>
       <c r="AD96">
-        <v>14.818181818181801</v>
+        <v>14.076923076923</v>
       </c>
       <c r="AE96">
         <v>13</v>
@@ -9598,7 +9619,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>4</v>
       </c>
@@ -9657,7 +9678,7 @@
         <v>914</v>
       </c>
       <c r="X97">
-        <v>17.743589743589698</v>
+        <v>17.243243243243199</v>
       </c>
       <c r="Y97">
         <v>28</v>
@@ -9675,7 +9696,7 @@
         <v>428</v>
       </c>
       <c r="AD97">
-        <v>18.8085106382978</v>
+        <v>15.636363636363599</v>
       </c>
       <c r="AE97">
         <v>11</v>
@@ -9693,7 +9714,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>5</v>
       </c>
@@ -9752,7 +9773,7 @@
         <v>652</v>
       </c>
       <c r="X98">
-        <v>3.2016806722689002</v>
+        <v>10.5185185185185</v>
       </c>
       <c r="Y98">
         <v>44</v>
@@ -9770,7 +9791,7 @@
         <v>214</v>
       </c>
       <c r="AD98">
-        <v>13.5744680851063</v>
+        <v>16.071428571428498</v>
       </c>
       <c r="AE98">
         <v>14</v>
@@ -9788,8 +9809,1352 @@
         <v>238</v>
       </c>
     </row>
+    <row r="100" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A100" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B100" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <f t="shared" ref="E100:H100" si="0">AVERAGE(E3:E10)</f>
+        <v>779.875</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="0"/>
+        <v>964.5</v>
+      </c>
+      <c r="G100">
+        <f t="shared" si="0"/>
+        <v>25.832230594401686</v>
+      </c>
+      <c r="I100">
+        <f>AVERAGE(I3:I10)</f>
+        <v>14.913891371495989</v>
+      </c>
+      <c r="J100">
+        <f t="shared" ref="J100:AI100" si="1">AVERAGE(J3:J10)</f>
+        <v>47</v>
+      </c>
+      <c r="K100">
+        <f t="shared" si="1"/>
+        <v>24.431869172494139</v>
+      </c>
+      <c r="L100">
+        <f t="shared" si="1"/>
+        <v>25.25</v>
+      </c>
+      <c r="M100">
+        <f t="shared" si="1"/>
+        <v>5.5176157007640807</v>
+      </c>
+      <c r="N100">
+        <f t="shared" si="1"/>
+        <v>649.125</v>
+      </c>
+      <c r="O100">
+        <f t="shared" si="1"/>
+        <v>10.603919577108469</v>
+      </c>
+      <c r="P100">
+        <f t="shared" si="1"/>
+        <v>69.875</v>
+      </c>
+      <c r="Q100">
+        <f t="shared" si="1"/>
+        <v>22.321658662456493</v>
+      </c>
+      <c r="R100">
+        <f t="shared" si="1"/>
+        <v>26.875</v>
+      </c>
+      <c r="S100">
+        <f t="shared" si="1"/>
+        <v>5.8108363884219125</v>
+      </c>
+      <c r="T100">
+        <f t="shared" si="1"/>
+        <v>579.375</v>
+      </c>
+      <c r="X100">
+        <f t="shared" si="1"/>
+        <v>13.451194638694629</v>
+      </c>
+      <c r="Y100">
+        <f t="shared" si="1"/>
+        <v>9.25</v>
+      </c>
+      <c r="Z100">
+        <f t="shared" si="1"/>
+        <v>15.834112394957963</v>
+      </c>
+      <c r="AA100">
+        <f t="shared" si="1"/>
+        <v>5.125</v>
+      </c>
+      <c r="AB100">
+        <f t="shared" si="1"/>
+        <v>5.4825548431899289</v>
+      </c>
+      <c r="AC100">
+        <f t="shared" si="1"/>
+        <v>130.75</v>
+      </c>
+      <c r="AD100">
+        <f t="shared" si="1"/>
+        <v>15.305505141192238</v>
+      </c>
+      <c r="AE100">
+        <f t="shared" si="1"/>
+        <v>48.125</v>
+      </c>
+      <c r="AF100">
+        <f t="shared" si="1"/>
+        <v>21.128205128205099</v>
+      </c>
+      <c r="AG100">
+        <f t="shared" si="1"/>
+        <v>18.125</v>
+      </c>
+      <c r="AH100">
+        <f t="shared" si="1"/>
+        <v>5.6337844910274768</v>
+      </c>
+      <c r="AI100">
+        <f t="shared" si="1"/>
+        <v>385.125</v>
+      </c>
+    </row>
+    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C101">
+        <v>0.03</v>
+      </c>
+      <c r="E101">
+        <f t="shared" ref="E101:H101" si="2">AVERAGE(E11:E18)</f>
+        <v>757</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="2"/>
+        <v>935.75</v>
+      </c>
+      <c r="G101">
+        <f t="shared" si="2"/>
+        <v>41.008429213829793</v>
+      </c>
+      <c r="I101">
+        <f>AVERAGE(I11:I18)</f>
+        <v>13.337684632306688</v>
+      </c>
+      <c r="J101">
+        <f t="shared" ref="J101:AI101" si="3">AVERAGE(J11:J18)</f>
+        <v>53.875</v>
+      </c>
+      <c r="K101">
+        <f t="shared" si="3"/>
+        <v>23.389032466706912</v>
+      </c>
+      <c r="L101">
+        <f t="shared" si="3"/>
+        <v>22.375</v>
+      </c>
+      <c r="M101">
+        <f t="shared" si="3"/>
+        <v>5.4624583531270581</v>
+      </c>
+      <c r="N101">
+        <f t="shared" si="3"/>
+        <v>542.625</v>
+      </c>
+      <c r="O101">
+        <f t="shared" si="3"/>
+        <v>11.706096089502671</v>
+      </c>
+      <c r="P101">
+        <f t="shared" si="3"/>
+        <v>72.625</v>
+      </c>
+      <c r="Q101">
+        <f t="shared" si="3"/>
+        <v>23.990827201868242</v>
+      </c>
+      <c r="R101">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="S101">
+        <f t="shared" si="3"/>
+        <v>5.5876436789374431</v>
+      </c>
+      <c r="T101">
+        <f t="shared" si="3"/>
+        <v>632.125</v>
+      </c>
+      <c r="X101">
+        <f t="shared" si="3"/>
+        <v>10.323492895119561</v>
+      </c>
+      <c r="Y101">
+        <f t="shared" si="3"/>
+        <v>21.125</v>
+      </c>
+      <c r="Z101">
+        <f t="shared" si="3"/>
+        <v>20.891882249694728</v>
+      </c>
+      <c r="AA101">
+        <f t="shared" si="3"/>
+        <v>8.375</v>
+      </c>
+      <c r="AB101">
+        <f t="shared" si="3"/>
+        <v>5.4728323138986479</v>
+      </c>
+      <c r="AC101">
+        <f t="shared" si="3"/>
+        <v>221</v>
+      </c>
+      <c r="AD101">
+        <f t="shared" si="3"/>
+        <v>15.457346439129941</v>
+      </c>
+      <c r="AE101">
+        <f t="shared" si="3"/>
+        <v>51.75</v>
+      </c>
+      <c r="AF101">
+        <f t="shared" si="3"/>
+        <v>23.077935606060574</v>
+      </c>
+      <c r="AG101">
+        <f t="shared" si="3"/>
+        <v>12.625</v>
+      </c>
+      <c r="AH101">
+        <f t="shared" si="3"/>
+        <v>5.6316021635186351</v>
+      </c>
+      <c r="AI101">
+        <f t="shared" si="3"/>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <v>0.06</v>
+      </c>
+      <c r="E102">
+        <f t="shared" ref="E102:H102" si="4">AVERAGE(E19:E26)</f>
+        <v>817.375</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="4"/>
+        <v>939.5</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="4"/>
+        <v>40.337864969251555</v>
+      </c>
+      <c r="I102">
+        <f>AVERAGE(I19:I26)</f>
+        <v>14.515829595075141</v>
+      </c>
+      <c r="J102">
+        <f t="shared" ref="J102:AI102" si="5">AVERAGE(J19:J26)</f>
+        <v>46.75</v>
+      </c>
+      <c r="K102">
+        <f t="shared" si="5"/>
+        <v>23.04366576218958</v>
+      </c>
+      <c r="L102">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="M102">
+        <f t="shared" si="5"/>
+        <v>5.4668900318396911</v>
+      </c>
+      <c r="N102">
+        <f t="shared" si="5"/>
+        <v>593.75</v>
+      </c>
+      <c r="O102">
+        <f t="shared" si="5"/>
+        <v>13.650125004160953</v>
+      </c>
+      <c r="P102">
+        <f t="shared" si="5"/>
+        <v>49.125</v>
+      </c>
+      <c r="Q102">
+        <f t="shared" si="5"/>
+        <v>24.7920951783723</v>
+      </c>
+      <c r="R102">
+        <f t="shared" si="5"/>
+        <v>23.625</v>
+      </c>
+      <c r="S102">
+        <f t="shared" si="5"/>
+        <v>5.5888735140629819</v>
+      </c>
+      <c r="T102">
+        <f t="shared" si="5"/>
+        <v>610</v>
+      </c>
+      <c r="X102">
+        <f t="shared" si="5"/>
+        <v>11.013839285714258</v>
+      </c>
+      <c r="Y102">
+        <f t="shared" si="5"/>
+        <v>15.125</v>
+      </c>
+      <c r="Z102">
+        <f t="shared" si="5"/>
+        <v>22.165567765567737</v>
+      </c>
+      <c r="AA102">
+        <f t="shared" si="5"/>
+        <v>7.5</v>
+      </c>
+      <c r="AB102">
+        <f t="shared" si="5"/>
+        <v>4.8150850407561556</v>
+      </c>
+      <c r="AC102">
+        <f t="shared" si="5"/>
+        <v>223.625</v>
+      </c>
+      <c r="AD102">
+        <f t="shared" si="5"/>
+        <v>19.372102753568235</v>
+      </c>
+      <c r="AE102">
+        <f t="shared" si="5"/>
+        <v>31.625</v>
+      </c>
+      <c r="AF102">
+        <f t="shared" si="5"/>
+        <v>26.030806616124686</v>
+      </c>
+      <c r="AG102">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="AH102">
+        <f t="shared" si="5"/>
+        <v>5.5691963621908158</v>
+      </c>
+      <c r="AI102">
+        <f t="shared" si="5"/>
+        <v>330.75</v>
+      </c>
+    </row>
+    <row r="103" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C103">
+        <v>0.1</v>
+      </c>
+      <c r="E103">
+        <f t="shared" ref="E103:H103" si="6">AVERAGE(E27:E34)</f>
+        <v>725</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="6"/>
+        <v>1002.25</v>
+      </c>
+      <c r="G103">
+        <f t="shared" si="6"/>
+        <v>31.496961851986537</v>
+      </c>
+      <c r="I103">
+        <f>AVERAGE(I27:I34)</f>
+        <v>10.048320069054949</v>
+      </c>
+      <c r="J103">
+        <f t="shared" ref="J103:AI103" si="7">AVERAGE(J27:J34)</f>
+        <v>59.125</v>
+      </c>
+      <c r="K103">
+        <f t="shared" si="7"/>
+        <v>22.247860413227684</v>
+      </c>
+      <c r="L103">
+        <f t="shared" si="7"/>
+        <v>25.125</v>
+      </c>
+      <c r="M103">
+        <f t="shared" si="7"/>
+        <v>5.3637503012159833</v>
+      </c>
+      <c r="N103">
+        <f t="shared" si="7"/>
+        <v>575.25</v>
+      </c>
+      <c r="O103">
+        <f t="shared" si="7"/>
+        <v>12.890554178020754</v>
+      </c>
+      <c r="P103">
+        <f t="shared" si="7"/>
+        <v>52.25</v>
+      </c>
+      <c r="Q103">
+        <f t="shared" si="7"/>
+        <v>24.074414159713022</v>
+      </c>
+      <c r="R103">
+        <f t="shared" si="7"/>
+        <v>24</v>
+      </c>
+      <c r="S103">
+        <f t="shared" si="7"/>
+        <v>5.6172006704177395</v>
+      </c>
+      <c r="T103">
+        <f t="shared" si="7"/>
+        <v>600.625</v>
+      </c>
+      <c r="X103">
+        <f t="shared" si="7"/>
+        <v>7.5826569264069086</v>
+      </c>
+      <c r="Y103">
+        <f t="shared" si="7"/>
+        <v>12.875</v>
+      </c>
+      <c r="Z103">
+        <f t="shared" si="7"/>
+        <v>16.37380050505049</v>
+      </c>
+      <c r="AA103">
+        <f t="shared" si="7"/>
+        <v>6.125</v>
+      </c>
+      <c r="AB103">
+        <f t="shared" si="7"/>
+        <v>4.0623650670080451</v>
+      </c>
+      <c r="AC103">
+        <f t="shared" si="7"/>
+        <v>149.75</v>
+      </c>
+      <c r="AD103">
+        <f t="shared" si="7"/>
+        <v>15.823777750909088</v>
+      </c>
+      <c r="AE103">
+        <f t="shared" si="7"/>
+        <v>37.125</v>
+      </c>
+      <c r="AF103">
+        <f t="shared" si="7"/>
+        <v>24.150932400932348</v>
+      </c>
+      <c r="AG103">
+        <f t="shared" si="7"/>
+        <v>15.375</v>
+      </c>
+      <c r="AH103">
+        <f t="shared" si="7"/>
+        <v>5.6796148486221458</v>
+      </c>
+      <c r="AI103">
+        <f t="shared" si="7"/>
+        <v>396.625</v>
+      </c>
+    </row>
+    <row r="104" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C104">
+        <v>0.5</v>
+      </c>
+      <c r="E104">
+        <f t="shared" ref="E104:H104" si="8">AVERAGE(E35:E42)</f>
+        <v>342.625</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="8"/>
+        <v>1083.125</v>
+      </c>
+      <c r="G104">
+        <f t="shared" si="8"/>
+        <v>14.920420643909239</v>
+      </c>
+      <c r="I104">
+        <f>AVERAGE(I35:I42)</f>
+        <v>4.4931352374740179</v>
+      </c>
+      <c r="X104">
+        <f t="shared" ref="J104:AI104" si="9">AVERAGE(X43:X50)</f>
+        <v>0.51762820512820495</v>
+      </c>
+      <c r="Y104">
+        <f t="shared" si="9"/>
+        <v>9.75</v>
+      </c>
+      <c r="Z104">
+        <f t="shared" si="9"/>
+        <v>1.744318181818175</v>
+      </c>
+      <c r="AA104">
+        <f t="shared" si="9"/>
+        <v>2.75</v>
+      </c>
+      <c r="AB104">
+        <f t="shared" si="9"/>
+        <v>0.74399612429926254</v>
+      </c>
+      <c r="AC104">
+        <f t="shared" si="9"/>
+        <v>42.125</v>
+      </c>
+      <c r="AD104">
+        <f t="shared" si="9"/>
+        <v>9.3510146103896048</v>
+      </c>
+      <c r="AE104">
+        <f t="shared" si="9"/>
+        <v>45</v>
+      </c>
+      <c r="AF104">
+        <f t="shared" si="9"/>
+        <v>23.372815893169076</v>
+      </c>
+      <c r="AG104">
+        <f t="shared" si="9"/>
+        <v>20.25</v>
+      </c>
+      <c r="AH104">
+        <f t="shared" si="9"/>
+        <v>5.5635858408285719</v>
+      </c>
+      <c r="AI104">
+        <f t="shared" si="9"/>
+        <v>475.375</v>
+      </c>
+    </row>
+    <row r="105" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C105">
+        <v>0.1</v>
+      </c>
+      <c r="E105">
+        <f t="shared" ref="E105:H105" si="10">AVERAGE(E43:E50)</f>
+        <v>236.5</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="10"/>
+        <v>1035</v>
+      </c>
+      <c r="G105">
+        <f t="shared" si="10"/>
+        <v>8.4081836327345254</v>
+      </c>
+      <c r="I105">
+        <f>AVERAGE(I43:I50)</f>
+        <v>3.0793971399535387</v>
+      </c>
+      <c r="J105">
+        <f>AVERAGE(J43:J50)</f>
+        <v>39.375</v>
+      </c>
+      <c r="K105">
+        <f>AVERAGE(K43:K50)</f>
+        <v>6.7361464548964465</v>
+      </c>
+      <c r="L105">
+        <f>AVERAGE(L43:L50)</f>
+        <v>16.125</v>
+      </c>
+      <c r="M105">
+        <f>AVERAGE(M43:M50)</f>
+        <v>5.4103520996246033</v>
+      </c>
+      <c r="N105">
+        <f>AVERAGE(N43:N50)</f>
+        <v>194.375</v>
+      </c>
+      <c r="O105">
+        <f>AVERAGE(O43:O50)</f>
+        <v>12.952429331883518</v>
+      </c>
+      <c r="P105">
+        <f>AVERAGE(P43:P50)</f>
+        <v>61.5</v>
+      </c>
+      <c r="Q105">
+        <f>AVERAGE(Q43:Q50)</f>
+        <v>24.029363312126449</v>
+      </c>
+      <c r="R105">
+        <f>AVERAGE(R43:R50)</f>
+        <v>23.625</v>
+      </c>
+      <c r="S105">
+        <f>AVERAGE(S43:S50)</f>
+        <v>5.5375682430759143</v>
+      </c>
+      <c r="T105">
+        <f>AVERAGE(T43:T50)</f>
+        <v>559.625</v>
+      </c>
+    </row>
+    <row r="106" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="X106">
+        <f t="shared" ref="J106:AI106" si="11">AVERAGE(X51:X58)</f>
+        <v>10.908985088985077</v>
+      </c>
+      <c r="Y106">
+        <f t="shared" si="11"/>
+        <v>26.875</v>
+      </c>
+      <c r="Z106">
+        <f t="shared" si="11"/>
+        <v>24.204727398205623</v>
+      </c>
+      <c r="AA106">
+        <f t="shared" si="11"/>
+        <v>15.25</v>
+      </c>
+      <c r="AB106">
+        <f t="shared" si="11"/>
+        <v>5.9465026278113688</v>
+      </c>
+      <c r="AC106">
+        <f t="shared" si="11"/>
+        <v>403.5</v>
+      </c>
+      <c r="AD106">
+        <f t="shared" si="11"/>
+        <v>7.7894736842105106</v>
+      </c>
+      <c r="AE106">
+        <f t="shared" si="11"/>
+        <v>11.5</v>
+      </c>
+      <c r="AF106">
+        <f t="shared" si="11"/>
+        <v>14.2144841269841</v>
+      </c>
+      <c r="AG106">
+        <f t="shared" si="11"/>
+        <v>5.875</v>
+      </c>
+      <c r="AH106">
+        <f t="shared" si="11"/>
+        <v>4.4923343926031132</v>
+      </c>
+      <c r="AI106">
+        <f t="shared" si="11"/>
+        <v>149.875</v>
+      </c>
+    </row>
+    <row r="107" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B107" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <f t="shared" ref="E107:H107" si="12">AVERAGE(E51:E58)</f>
+        <v>1043</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="12"/>
+        <v>771.375</v>
+      </c>
+      <c r="G107">
+        <f t="shared" si="12"/>
+        <v>71.089942423277805</v>
+      </c>
+      <c r="I107">
+        <f>AVERAGE(I51:I58)</f>
+        <v>18.880415263037516</v>
+      </c>
+      <c r="J107">
+        <f>AVERAGE(J51:J58)</f>
+        <v>45.125</v>
+      </c>
+      <c r="K107">
+        <f>AVERAGE(K51:K58)</f>
+        <v>26.302746390122984</v>
+      </c>
+      <c r="L107">
+        <f>AVERAGE(L51:L58)</f>
+        <v>25.25</v>
+      </c>
+      <c r="M107">
+        <f>AVERAGE(M51:M58)</f>
+        <v>5.9918680483855358</v>
+      </c>
+      <c r="N107">
+        <f>AVERAGE(N51:N58)</f>
+        <v>639.5</v>
+      </c>
+      <c r="O107">
+        <f>AVERAGE(O51:O58)</f>
+        <v>15.656545511482884</v>
+      </c>
+      <c r="P107">
+        <f>AVERAGE(P51:P58)</f>
+        <v>46.875</v>
+      </c>
+      <c r="Q107">
+        <f>AVERAGE(Q51:Q58)</f>
+        <v>25.792057049230898</v>
+      </c>
+      <c r="R107">
+        <f>AVERAGE(R51:R58)</f>
+        <v>23.5</v>
+      </c>
+      <c r="S107">
+        <f>AVERAGE(S51:S58)</f>
+        <v>6.0663052538155489</v>
+      </c>
+      <c r="T107">
+        <f>AVERAGE(T51:T58)</f>
+        <v>621.5</v>
+      </c>
+      <c r="X107">
+        <f t="shared" ref="J107:AI107" si="13">AVERAGE(X59:X66)</f>
+        <v>11.410463360171001</v>
+      </c>
+      <c r="Y107">
+        <f t="shared" si="13"/>
+        <v>30.375</v>
+      </c>
+      <c r="Z107">
+        <f t="shared" si="13"/>
+        <v>24.990766749590225</v>
+      </c>
+      <c r="AA107">
+        <f t="shared" si="13"/>
+        <v>17.875</v>
+      </c>
+      <c r="AB107">
+        <f t="shared" si="13"/>
+        <v>5.9347698679543894</v>
+      </c>
+      <c r="AC107">
+        <f t="shared" si="13"/>
+        <v>474.625</v>
+      </c>
+      <c r="AD107">
+        <f t="shared" si="13"/>
+        <v>17.668181818181814</v>
+      </c>
+      <c r="AE107">
+        <f t="shared" si="13"/>
+        <v>4.125</v>
+      </c>
+      <c r="AF107">
+        <f t="shared" si="13"/>
+        <v>19.075892857142851</v>
+      </c>
+      <c r="AG107">
+        <f t="shared" si="13"/>
+        <v>2.625</v>
+      </c>
+      <c r="AH107">
+        <f t="shared" si="13"/>
+        <v>5.2447079665566614</v>
+      </c>
+      <c r="AI107">
+        <f t="shared" si="13"/>
+        <v>105.875</v>
+      </c>
+    </row>
+    <row r="108" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C108">
+        <v>0.03</v>
+      </c>
+      <c r="E108">
+        <f t="shared" ref="E108:H108" si="14">AVERAGE(E59:E66)</f>
+        <v>1125.875</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="14"/>
+        <v>780.875</v>
+      </c>
+      <c r="G108">
+        <f t="shared" si="14"/>
+        <v>81.844009668033095</v>
+      </c>
+      <c r="I108">
+        <f>AVERAGE(I59:I66)</f>
+        <v>17.182772409112523</v>
+      </c>
+      <c r="J108">
+        <f>AVERAGE(J59:J66)</f>
+        <v>43.625</v>
+      </c>
+      <c r="K108">
+        <f>AVERAGE(K59:K66)</f>
+        <v>26.49937904136533</v>
+      </c>
+      <c r="L108">
+        <f>AVERAGE(L59:L66)</f>
+        <v>24.375</v>
+      </c>
+      <c r="M108">
+        <f>AVERAGE(M59:M66)</f>
+        <v>5.9384964260911932</v>
+      </c>
+      <c r="N108">
+        <f>AVERAGE(N59:N66)</f>
+        <v>651.25</v>
+      </c>
+      <c r="O108">
+        <f>AVERAGE(O59:O66)</f>
+        <v>19.806393625681626</v>
+      </c>
+      <c r="P108">
+        <f>AVERAGE(P59:P66)</f>
+        <v>38.5</v>
+      </c>
+      <c r="Q108">
+        <f>AVERAGE(Q59:Q66)</f>
+        <v>28.419496047430801</v>
+      </c>
+      <c r="R108">
+        <f>AVERAGE(R59:R66)</f>
+        <v>23</v>
+      </c>
+      <c r="S108">
+        <f>AVERAGE(S59:S66)</f>
+        <v>6.0559069966601191</v>
+      </c>
+      <c r="T108">
+        <f>AVERAGE(T59:T66)</f>
+        <v>675</v>
+      </c>
+      <c r="X108">
+        <f t="shared" ref="J108:AI108" si="15">AVERAGE(X67:X74)</f>
+        <v>14.137649930451142</v>
+      </c>
+      <c r="Y108">
+        <f t="shared" si="15"/>
+        <v>22.25</v>
+      </c>
+      <c r="Z108">
+        <f t="shared" si="15"/>
+        <v>29.119662838988461</v>
+      </c>
+      <c r="AA108">
+        <f t="shared" si="15"/>
+        <v>13.625</v>
+      </c>
+      <c r="AB108">
+        <f t="shared" si="15"/>
+        <v>5.9957647437090857</v>
+      </c>
+      <c r="AC108">
+        <f t="shared" si="15"/>
+        <v>450</v>
+      </c>
+      <c r="AD108">
+        <f t="shared" si="15"/>
+        <v>12.449878372401562</v>
+      </c>
+      <c r="AE108">
+        <f t="shared" si="15"/>
+        <v>6.625</v>
+      </c>
+      <c r="AF108">
+        <f t="shared" si="15"/>
+        <v>17.4722222222222</v>
+      </c>
+      <c r="AG108">
+        <f t="shared" si="15"/>
+        <v>4.5</v>
+      </c>
+      <c r="AH108">
+        <f t="shared" si="15"/>
+        <v>4.817502511729181</v>
+      </c>
+      <c r="AI108">
+        <f t="shared" si="15"/>
+        <v>130.75</v>
+      </c>
+    </row>
+    <row r="109" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C109">
+        <v>0.06</v>
+      </c>
+      <c r="E109">
+        <f t="shared" ref="E109:H109" si="16">AVERAGE(E67:E74)</f>
+        <v>1094</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="16"/>
+        <v>784.375</v>
+      </c>
+      <c r="G109">
+        <f t="shared" si="16"/>
+        <v>72.623029365208595</v>
+      </c>
+      <c r="I109">
+        <f>AVERAGE(I67:I74)</f>
+        <v>17.933431598924127</v>
+      </c>
+      <c r="J109">
+        <f>AVERAGE(J67:J74)</f>
+        <v>44.25</v>
+      </c>
+      <c r="K109">
+        <f>AVERAGE(K67:K74)</f>
+        <v>27.58288514022205</v>
+      </c>
+      <c r="L109">
+        <f>AVERAGE(L67:L74)</f>
+        <v>22.875</v>
+      </c>
+      <c r="M109">
+        <f>AVERAGE(M67:M74)</f>
+        <v>6.0123002183028875</v>
+      </c>
+      <c r="N109">
+        <f>AVERAGE(N67:N74)</f>
+        <v>646.5</v>
+      </c>
+      <c r="O109">
+        <f>AVERAGE(O67:O74)</f>
+        <v>17.280293032609414</v>
+      </c>
+      <c r="P109">
+        <f>AVERAGE(P67:P74)</f>
+        <v>41.75</v>
+      </c>
+      <c r="Q109">
+        <f>AVERAGE(Q67:Q74)</f>
+        <v>26.785015935151762</v>
+      </c>
+      <c r="R109">
+        <f>AVERAGE(R67:R74)</f>
+        <v>23.625</v>
+      </c>
+      <c r="S109">
+        <f>AVERAGE(S67:S74)</f>
+        <v>6.1880837849525019</v>
+      </c>
+      <c r="T109">
+        <f>AVERAGE(T67:T74)</f>
+        <v>653.625</v>
+      </c>
+      <c r="X109">
+        <f t="shared" ref="J109:AI109" si="17">AVERAGE(X75:X82)</f>
+        <v>12.567562138878692</v>
+      </c>
+      <c r="Y109">
+        <f t="shared" si="17"/>
+        <v>38.25</v>
+      </c>
+      <c r="Z109">
+        <f t="shared" si="17"/>
+        <v>25.271300667482837</v>
+      </c>
+      <c r="AA109">
+        <f t="shared" si="17"/>
+        <v>19.625</v>
+      </c>
+      <c r="AB109">
+        <f t="shared" si="17"/>
+        <v>6.0598078282861536</v>
+      </c>
+      <c r="AC109">
+        <f t="shared" si="17"/>
+        <v>518.75</v>
+      </c>
+      <c r="AD109">
+        <f t="shared" si="17"/>
+        <v>9.9416666666666504</v>
+      </c>
+      <c r="AE109">
+        <f t="shared" si="17"/>
+        <v>2.25</v>
+      </c>
+      <c r="AF109">
+        <f t="shared" si="17"/>
+        <v>13.614583333333325</v>
+      </c>
+      <c r="AG109">
+        <f t="shared" si="17"/>
+        <v>1.5</v>
+      </c>
+      <c r="AH109">
+        <f t="shared" si="17"/>
+        <v>3.8815357000131874</v>
+      </c>
+      <c r="AI109">
+        <f t="shared" si="17"/>
+        <v>56.875</v>
+      </c>
+    </row>
+    <row r="110" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C110">
+        <v>0.1</v>
+      </c>
+      <c r="E110">
+        <f t="shared" ref="E110:H110" si="18">AVERAGE(E75:E82)</f>
+        <v>1226</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="18"/>
+        <v>738</v>
+      </c>
+      <c r="G110">
+        <f t="shared" si="18"/>
+        <v>89.251347141871193</v>
+      </c>
+      <c r="I110">
+        <f>AVERAGE(I75:I82)</f>
+        <v>20.077421257561568</v>
+      </c>
+      <c r="J110">
+        <f>AVERAGE(J75:J82)</f>
+        <v>40</v>
+      </c>
+      <c r="K110">
+        <f>AVERAGE(K75:K82)</f>
+        <v>29.464245195223413</v>
+      </c>
+      <c r="L110">
+        <f>AVERAGE(L75:L82)</f>
+        <v>23.125</v>
+      </c>
+      <c r="M110">
+        <f>AVERAGE(M75:M82)</f>
+        <v>6.0894418804810755</v>
+      </c>
+      <c r="N110">
+        <f>AVERAGE(N75:N82)</f>
+        <v>707.25</v>
+      </c>
+      <c r="O110">
+        <f>AVERAGE(O75:O82)</f>
+        <v>18.731188594690721</v>
+      </c>
+      <c r="P110">
+        <f>AVERAGE(P75:P82)</f>
+        <v>38.5</v>
+      </c>
+      <c r="Q110">
+        <f>AVERAGE(Q75:Q82)</f>
+        <v>28.182385323010273</v>
+      </c>
+      <c r="R110">
+        <f>AVERAGE(R75:R82)</f>
+        <v>23.625</v>
+      </c>
+      <c r="S110">
+        <f>AVERAGE(S75:S82)</f>
+        <v>6.2927502888410549</v>
+      </c>
+      <c r="T110">
+        <f>AVERAGE(T75:T82)</f>
+        <v>681.125</v>
+      </c>
+      <c r="X110">
+        <f t="shared" ref="J110:AI110" si="19">AVERAGE(X83:X90)</f>
+        <v>13.3667081529581</v>
+      </c>
+      <c r="Y110">
+        <f t="shared" si="19"/>
+        <v>41.875</v>
+      </c>
+      <c r="Z110">
+        <f t="shared" si="19"/>
+        <v>14.972064393939386</v>
+      </c>
+      <c r="AA110">
+        <f t="shared" si="19"/>
+        <v>17.5</v>
+      </c>
+      <c r="AB110">
+        <f t="shared" si="19"/>
+        <v>5.1162189655465502</v>
+      </c>
+      <c r="AC110">
+        <f t="shared" si="19"/>
+        <v>307.125</v>
+      </c>
+      <c r="AD110">
+        <f t="shared" si="19"/>
+        <v>7.2635364299678651</v>
+      </c>
+      <c r="AE110">
+        <f t="shared" si="19"/>
+        <v>15.875</v>
+      </c>
+      <c r="AF110">
+        <f t="shared" si="19"/>
+        <v>17.650035014005574</v>
+      </c>
+      <c r="AG110">
+        <f t="shared" si="19"/>
+        <v>6.25</v>
+      </c>
+      <c r="AH110">
+        <f t="shared" si="19"/>
+        <v>5.4746302113265903</v>
+      </c>
+      <c r="AI110">
+        <f t="shared" si="19"/>
+        <v>175.125</v>
+      </c>
+    </row>
+    <row r="111" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C111">
+        <v>0.5</v>
+      </c>
+      <c r="E111">
+        <f t="shared" ref="E111:H111" si="20">AVERAGE(E83:E90)</f>
+        <v>842.125</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="20"/>
+        <v>856.625</v>
+      </c>
+      <c r="G111">
+        <f t="shared" si="20"/>
+        <v>59.104140946707361</v>
+      </c>
+      <c r="I111">
+        <f>AVERAGE(I83:I90)</f>
+        <v>8.2459955685795823</v>
+      </c>
+      <c r="J111">
+        <f>AVERAGE(J83:J90)</f>
+        <v>79.75</v>
+      </c>
+      <c r="K111">
+        <f>AVERAGE(K83:K90)</f>
+        <v>16.237695638416632</v>
+      </c>
+      <c r="L111">
+        <f>AVERAGE(L83:L90)</f>
+        <v>35.5</v>
+      </c>
+      <c r="M111">
+        <f>AVERAGE(M83:M90)</f>
+        <v>5.9564192901602002</v>
+      </c>
+      <c r="N111">
+        <f>AVERAGE(N83:N90)</f>
+        <v>534.875</v>
+      </c>
+      <c r="O111">
+        <f>AVERAGE(O83:O90)</f>
+        <v>19.027899101559797</v>
+      </c>
+      <c r="P111">
+        <f>AVERAGE(P83:P90)</f>
+        <v>38.375</v>
+      </c>
+      <c r="Q111">
+        <f>AVERAGE(Q83:Q90)</f>
+        <v>28.825954968944064</v>
+      </c>
+      <c r="R111">
+        <f>AVERAGE(R83:R90)</f>
+        <v>22.875</v>
+      </c>
+      <c r="S111">
+        <f>AVERAGE(S83:S90)</f>
+        <v>6.3327041825051111</v>
+      </c>
+      <c r="T111">
+        <f>AVERAGE(T83:T90)</f>
+        <v>681.375</v>
+      </c>
+      <c r="X111">
+        <f t="shared" ref="J111:AI111" si="21">AVERAGE(X91:X98)</f>
+        <v>12.891524666875316</v>
+      </c>
+      <c r="Y111">
+        <f t="shared" si="21"/>
+        <v>28.875</v>
+      </c>
+      <c r="Z111">
+        <f t="shared" si="21"/>
+        <v>17.09196047008545</v>
+      </c>
+      <c r="AA111">
+        <f t="shared" si="21"/>
+        <v>12.75</v>
+      </c>
+      <c r="AB111">
+        <f t="shared" si="21"/>
+        <v>5.1673841648365375</v>
+      </c>
+      <c r="AC111">
+        <f t="shared" si="21"/>
+        <v>276.5</v>
+      </c>
+      <c r="AD111">
+        <f t="shared" si="21"/>
+        <v>14.849081474081434</v>
+      </c>
+      <c r="AE111">
+        <f t="shared" si="21"/>
+        <v>17.625</v>
+      </c>
+      <c r="AF111">
+        <f t="shared" si="21"/>
+        <v>23.817747968405836</v>
+      </c>
+      <c r="AG111">
+        <f t="shared" si="21"/>
+        <v>9.125</v>
+      </c>
+      <c r="AH111">
+        <f t="shared" si="21"/>
+        <v>6.0003249547381925</v>
+      </c>
+      <c r="AI111">
+        <f t="shared" si="21"/>
+        <v>230.25</v>
+      </c>
+    </row>
+    <row r="112" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="C112">
+        <v>0.1</v>
+      </c>
+      <c r="E112">
+        <f t="shared" ref="E112:H112" si="22">AVERAGE(E91:E98)</f>
+        <v>887.625</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="22"/>
+        <v>913.25</v>
+      </c>
+      <c r="G112">
+        <f t="shared" si="22"/>
+        <v>55.041854353595056</v>
+      </c>
+      <c r="I112">
+        <f>AVERAGE(I91:I98)</f>
+        <v>11.036269810182503</v>
+      </c>
+      <c r="J112">
+        <f>AVERAGE(J91:J98)</f>
+        <v>75.125</v>
+      </c>
+      <c r="K112">
+        <f>AVERAGE(K91:K98)</f>
+        <v>20.329766139657423</v>
+      </c>
+      <c r="L112">
+        <f>AVERAGE(L91:L98)</f>
+        <v>30.625</v>
+      </c>
+      <c r="M112">
+        <f>AVERAGE(M91:M98)</f>
+        <v>7.8104327545096197</v>
+      </c>
+      <c r="N112">
+        <f>AVERAGE(N91:N98)</f>
+        <v>611.125</v>
+      </c>
+      <c r="O112">
+        <f>AVERAGE(O91:O98)</f>
+        <v>14.835116675019536</v>
+      </c>
+      <c r="P112">
+        <f>AVERAGE(P91:P98)</f>
+        <v>53.625</v>
+      </c>
+      <c r="Q112">
+        <f>AVERAGE(Q91:Q98)</f>
+        <v>27.453932558224139</v>
+      </c>
+      <c r="R112">
+        <f>AVERAGE(R91:R98)</f>
+        <v>24.125</v>
+      </c>
+      <c r="S112">
+        <f>AVERAGE(S91:S98)</f>
+        <v>6.8963185956441002</v>
+      </c>
+      <c r="T112">
+        <f>AVERAGE(T91:T98)</f>
+        <v>683</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B114" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C115">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C116">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C117">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C118">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C119">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B121" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C122">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C123">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C124">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C125">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C126">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:T98" xr:uid="{C0F397ED-332E-4C31-A79E-0DDC00B2F78D}"/>
+  <autoFilter ref="A2:T98"/>
   <sortState ref="A3:F98">
     <sortCondition ref="B3:B98"/>
     <sortCondition ref="C3:C98"/>

</xml_diff>